<commit_message>
Fix issues found during tests
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_8_10.xlsx
+++ b/templates/NHWA_Module_8_10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46688AA-9A90-4605-969A-4871503B8E99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8F78F1-C2EE-4169-B4C5-BB06FA3E12CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="zzB/EG68cBLCavBKifLXLU9cHtkByNHDxKw6TGAOmH0Xqt9eEqslmxhiS3RNT5/yg3W/p9o2mkoBv+FWclA2/Q==" workbookSaltValue="AdDK0FT/Ht0UdvlaiqFRnA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="794">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -2393,6 +2393,21 @@
   </si>
   <si>
     <t xml:space="preserve">YES </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Developed</t>
+  </si>
+  <si>
+    <t>Demonstrated</t>
+  </si>
+  <si>
+    <t>Sustainable</t>
   </si>
 </sst>
 </file>
@@ -2563,9 +2578,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -2625,9 +2637,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2640,14 +2649,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2660,7 +2677,7 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2707,55 +2724,63 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$11" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$12" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$13" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$10" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$14" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$15" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$16" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$V$22" fmlaRange="$V$15:$V$20" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$W$22" fmlaRange="$V$15:$V$20" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$9" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$11" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$12" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$13" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$10" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$9" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$11" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$12" fmlaRange="$N$3:$N$6" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2842,6 +2867,122 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2055" name="Drop Down 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2055"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2056" name="Drop Down 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2056"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3983,16 +4124,15 @@
     <col min="8" max="8" width="15.5703125" style="4" customWidth="1"/>
     <col min="9" max="9" width="16" style="4" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4" customWidth="1"/>
-    <col min="12" max="15" width="9.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="15" width="9.140625" style="4" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" style="4" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" style="4" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="16.28515625" style="4" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="4" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="12.140625" style="4" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="9.7109375" style="4" hidden="1" customWidth="1"/>
-    <col min="22" max="33" width="9.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="34" max="35" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="22" max="34" width="9.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="9.140625" style="4" customWidth="1"/>
     <col min="36" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -4018,7 +4158,7 @@
       <c r="R1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>760</v>
       </c>
       <c r="W1" s="1"/>
@@ -4058,7 +4198,7 @@
       <c r="R2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
-      <c r="V2" s="9" t="e">
+      <c r="V2" s="8" t="e">
         <f>VLOOKUP(V1,Y2:AB250,2,0)</f>
         <v>#N/A</v>
       </c>
@@ -4099,20 +4239,20 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
       <c r="Y3" s="4" t="s">
         <v>6</v>
       </c>
@@ -4139,20 +4279,20 @@
       </c>
     </row>
     <row r="4" spans="2:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="31" t="str">
+      <c r="E4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="29" t="str">
         <f>IFERROR(VLOOKUP(V1,Y2:AB249,4,0),"")</f>
         <v/>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="29"/>
+      <c r="I4" s="28"/>
       <c r="Y4" s="4" t="s">
         <v>7</v>
       </c>
@@ -4179,8 +4319,8 @@
       </c>
     </row>
     <row r="5" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4240,12 +4380,12 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
-      <c r="I6" s="15"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
+      <c r="I6" s="14"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
       <c r="S6" s="39"/>
       <c r="T6" s="39"/>
       <c r="V6" s="4" t="s">
@@ -4284,18 +4424,18 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
-      <c r="I7" s="15"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="V7" s="10" t="s">
+      <c r="I7" s="14"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="V7" s="9" t="s">
         <v>758</v>
       </c>
-      <c r="W7" s="10"/>
+      <c r="W7" s="9"/>
       <c r="Y7" s="4" t="s">
         <v>11</v>
       </c>
@@ -4322,23 +4462,23 @@
       </c>
     </row>
     <row r="8" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
-        <v>1</v>
-      </c>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="15">
+        <v>1</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>783</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="36"/>
       <c r="F8" s="36"/>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
-      <c r="I8" s="15"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
+      <c r="I8" s="14"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
       <c r="Y8" s="4" t="s">
         <v>205</v>
       </c>
@@ -4365,23 +4505,23 @@
       </c>
     </row>
     <row r="9" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>2</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>784</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
       <c r="G9" s="36"/>
       <c r="H9" s="36"/>
-      <c r="I9" s="15"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
+      <c r="I9" s="14"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
       <c r="Y9" s="4" t="s">
         <v>12</v>
       </c>
@@ -4408,29 +4548,29 @@
       </c>
     </row>
     <row r="10" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>3</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>785</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
-      <c r="I10" s="15"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="V10" s="10">
-        <v>1</v>
-      </c>
-      <c r="W10" s="10"/>
+      <c r="I10" s="14"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="V10" s="9">
+        <v>1</v>
+      </c>
+      <c r="W10" s="9"/>
       <c r="Y10" s="4" t="s">
         <v>13</v>
       </c>
@@ -4457,27 +4597,27 @@
       </c>
     </row>
     <row r="11" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>4</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>765</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="35"/>
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
-      <c r="I11" s="15"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
+      <c r="I11" s="14"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
       <c r="Y11" s="4" t="s">
         <v>14</v>
       </c>
@@ -4504,32 +4644,32 @@
       </c>
     </row>
     <row r="12" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>5</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>786</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="38"/>
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
       <c r="H12" s="38"/>
-      <c r="I12" s="15"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
+      <c r="I12" s="14"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
       <c r="U12" s="4" t="s">
         <v>757</v>
       </c>
-      <c r="V12" s="10" t="s">
+      <c r="V12" s="9" t="s">
         <v>787</v>
       </c>
-      <c r="W12" s="10" t="s">
+      <c r="W12" s="9" t="s">
         <v>758</v>
       </c>
       <c r="Y12" s="4" t="s">
@@ -4558,25 +4698,25 @@
       </c>
     </row>
     <row r="13" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <v>6</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>763</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="17"/>
       <c r="E13" s="37"/>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
-      <c r="I13" s="15"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
+      <c r="I13" s="14"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
       <c r="U13" s="4" t="str">
         <f>IF($V$10=2,"True","")</f>
         <v/>
@@ -4615,27 +4755,27 @@
       </c>
     </row>
     <row r="14" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <v>7</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>764</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
-      <c r="I14" s="15"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
+      <c r="I14" s="14"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
       <c r="Y14" s="4" t="s">
         <v>220</v>
       </c>
@@ -4662,25 +4802,29 @@
       </c>
     </row>
     <row r="15" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>8</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>765</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
-      <c r="I15" s="15"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="V15" s="4" t="str">
+        <f>""</f>
+        <v/>
+      </c>
       <c r="Y15" s="4" t="s">
         <v>15</v>
       </c>
@@ -4707,15 +4851,18 @@
       </c>
     </row>
     <row r="16" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="V16" s="4" t="s">
+        <v>789</v>
+      </c>
       <c r="Y16" s="4" t="s">
         <v>16</v>
       </c>
@@ -4742,8 +4889,11 @@
       </c>
     </row>
     <row r="17" spans="8:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="V17" s="4" t="s">
+        <v>790</v>
+      </c>
       <c r="Y17" s="4" t="s">
         <v>17</v>
       </c>
@@ -4770,8 +4920,11 @@
       </c>
     </row>
     <row r="18" spans="8:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="V18" s="4" t="s">
+        <v>791</v>
+      </c>
       <c r="Y18" s="4" t="s">
         <v>18</v>
       </c>
@@ -4798,6 +4951,9 @@
       </c>
     </row>
     <row r="19" spans="8:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="4" t="s">
+        <v>792</v>
+      </c>
       <c r="Y19" s="4" t="s">
         <v>19</v>
       </c>
@@ -4824,6 +4980,9 @@
       </c>
     </row>
     <row r="20" spans="8:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="4" t="s">
+        <v>793</v>
+      </c>
       <c r="Y20" s="4" t="s">
         <v>20</v>
       </c>
@@ -4876,6 +5035,12 @@
       </c>
     </row>
     <row r="22" spans="8:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V22" s="9">
+        <v>1</v>
+      </c>
+      <c r="W22" s="9">
+        <v>1</v>
+      </c>
       <c r="Y22" s="4" t="s">
         <v>22</v>
       </c>
@@ -4902,6 +5067,14 @@
       </c>
     </row>
     <row r="23" spans="8:31" x14ac:dyDescent="0.25">
+      <c r="V23" s="4" t="str">
+        <f ca="1">INDIRECT(ADDRESS(ROW(V15)+V22-1,COLUMN(V15)))</f>
+        <v/>
+      </c>
+      <c r="W23" s="4" t="str">
+        <f ca="1">INDIRECT(ADDRESS(ROW(V15)+W22-1,COLUMN(V15)))</f>
+        <v/>
+      </c>
       <c r="Y23" s="4" t="s">
         <v>23</v>
       </c>
@@ -10858,7 +11031,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/BfU4acKoReI7WsfaoCMlDvbWGO7S/XFv7106xJkqSZ79C/ENIxss7U0mjqWpoSXZocH5vlpiEeM8Q1AHVTrDA==" saltValue="nh0Fk2seh5XbtMT9I0dFBw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ayvvL4B0rTmiFtoL19BmlgzP+5zKbPPR9GO1TrkLAaTIwNt3IeEuZgbylSBRZXxwEKB3feYmUw1a6fmT88kPKQ==" saltValue="DJoPVZM/QTKyvsO1jcr2Qg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="I4 Q8:R16 F8:P10 F14:P14 G11:P13 H15:P15 D17:G17 D21:G21 F13" name="Range1"/>
     <protectedRange sqref="D10:E13" name="Range1_1"/>
@@ -10932,6 +11105,50 @@
         </control>
       </mc:Choice>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2055" r:id="rId7" name="Drop Down 7">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2056" r:id="rId8" name="Drop Down 8">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+    </mc:AlternateContent>
   </controls>
 </worksheet>
 </file>
@@ -10939,7 +11156,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:S19"/>
+  <dimension ref="B1:T19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E9" sqref="E9:I9"/>
@@ -10959,8 +11176,8 @@
     <col min="11" max="11" width="11.7109375" style="4" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" style="4" hidden="1" customWidth="1"/>
-    <col min="14" max="19" width="9.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="4" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -10995,61 +11212,62 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="10" t="e">
+      <c r="N2" s="9" t="e">
+        <f>'M08 - Skill mix composition'!V2</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="10"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="31" t="str">
+      <c r="C4" s="29" t="str">
         <f>'M08 - Skill mix composition'!V1</f>
         <v/>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="31" t="str">
+      <c r="E4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="29" t="str">
         <f>'M08 - Skill mix composition'!F4</f>
         <v/>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="29">
         <f>'M08 - Skill mix composition'!I4</f>
         <v>0</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>757</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>787</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="L6" s="5"/>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>758</v>
       </c>
     </row>
@@ -11070,7 +11288,7 @@
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>
-      <c r="N7" s="10"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" spans="2:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="40"/>
@@ -11081,7 +11299,7 @@
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" s="40"/>
-      <c r="N8" s="10"/>
+      <c r="N8" s="9"/>
       <c r="Q8" s="4" t="s">
         <v>757</v>
       </c>
@@ -11093,22 +11311,22 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
-        <v>1</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>768</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
       <c r="I9" s="42"/>
-      <c r="N9" s="10">
-        <v>1</v>
-      </c>
-      <c r="O9" s="10"/>
+      <c r="N9" s="9">
+        <v>1</v>
+      </c>
+      <c r="O9" s="9"/>
       <c r="Q9" s="4" t="str">
         <f>IF($N9=2,"True","")</f>
         <v/>
@@ -11123,22 +11341,22 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>2</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>769</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
-      <c r="N10" s="10">
-        <v>1</v>
-      </c>
-      <c r="O10" s="10"/>
+      <c r="N10" s="9">
+        <v>1</v>
+      </c>
+      <c r="O10" s="9"/>
       <c r="Q10" s="4" t="str">
         <f>IF($N10=2,"True","")</f>
         <v/>
@@ -11153,22 +11371,22 @@
       </c>
     </row>
     <row r="11" spans="2:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>3</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>770</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="42"/>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
-      <c r="N11" s="10">
-        <v>1</v>
-      </c>
-      <c r="O11" s="10"/>
+      <c r="N11" s="9">
+        <v>1</v>
+      </c>
+      <c r="O11" s="9"/>
       <c r="Q11" s="4" t="str">
         <f>IF($N11=2,"True","")</f>
         <v/>
@@ -11183,22 +11401,22 @@
       </c>
     </row>
     <row r="12" spans="2:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>4</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>771</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="42"/>
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
       <c r="H12" s="42"/>
       <c r="I12" s="42"/>
-      <c r="N12" s="10">
-        <v>1</v>
-      </c>
-      <c r="O12" s="10"/>
+      <c r="N12" s="9">
+        <v>1</v>
+      </c>
+      <c r="O12" s="9"/>
       <c r="Q12" s="4" t="str">
         <f>IF($N12=2,"True","")</f>
         <v/>
@@ -11213,22 +11431,22 @@
       </c>
     </row>
     <row r="13" spans="2:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <v>5</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>772</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
       <c r="H13" s="42"/>
       <c r="I13" s="42"/>
-      <c r="N13" s="10">
-        <v>1</v>
-      </c>
-      <c r="O13" s="10"/>
+      <c r="N13" s="9">
+        <v>1</v>
+      </c>
+      <c r="O13" s="9"/>
       <c r="Q13" s="4" t="str">
         <f>IF($N13=2,"True","")</f>
         <v/>
@@ -11248,11 +11466,11 @@
     <row r="17" spans="14:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="14:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="a1UZUhd5qshf6UwsWA7udpvHhl45OYCMXG55fx6LBgePOrDbSaRsxxdrRC2OkAlSp/6tJk1rxLBlaY3steUfmA==" saltValue="qZwt9mmFf+/Ytge+V/7/RA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="OEvvRjWpKbFC0jARZBSL+ULn5yEhPQzieqzguPUHK0SM5DBJVo007Oj/Yo6NQcHhcZpMEDsduY26Nam8tHTTFQ==" saltValue="zQBbEZUen1o0bsK22UMd/w==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="D19" name="Range1_1_1"/>
     <protectedRange sqref="D9:D11 D14" name="Range1_2"/>
@@ -11417,7 +11635,7 @@
     <col min="12" max="12" width="9.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="14" max="20" width="9.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="4" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -11452,48 +11670,49 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="10" t="e">
+      <c r="N2" s="9" t="e">
+        <f>'M08 - Skill mix composition'!V2</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="10"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="31" t="str">
+      <c r="C4" s="29" t="str">
         <f>'M08 - Skill mix composition'!V1</f>
         <v/>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="31" t="str">
+      <c r="E4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="29" t="str">
         <f>'M08 - Skill mix composition'!F4</f>
         <v/>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="29">
         <f>'M08 - Skill mix composition'!I4</f>
         <v>0</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>757</v>
       </c>
     </row>
@@ -11506,7 +11725,7 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="L6" s="5"/>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>758</v>
       </c>
     </row>
@@ -11526,7 +11745,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
-      <c r="N7" s="10"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" spans="2:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="40"/>
@@ -11536,7 +11755,7 @@
       <c r="F8" s="40"/>
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
-      <c r="N8" s="10"/>
+      <c r="N8" s="9"/>
       <c r="Q8" s="4" t="s">
         <v>788</v>
       </c>
@@ -11548,21 +11767,21 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
-        <v>1</v>
-      </c>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+      <c r="C9" s="31" t="s">
         <v>774</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
-      <c r="N9" s="10">
-        <v>1</v>
-      </c>
-      <c r="O9" s="10"/>
+      <c r="N9" s="9">
+        <v>1</v>
+      </c>
+      <c r="O9" s="9"/>
       <c r="Q9" s="4" t="str">
         <f t="shared" ref="Q9:Q16" si="0">IF($N9=2,"True","")</f>
         <v/>
@@ -11577,21 +11796,21 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>2</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="31" t="s">
         <v>775</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
       <c r="H10" s="42"/>
-      <c r="N10" s="10">
-        <v>1</v>
-      </c>
-      <c r="O10" s="10"/>
+      <c r="N10" s="9">
+        <v>1</v>
+      </c>
+      <c r="O10" s="9"/>
       <c r="Q10" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -11606,21 +11825,21 @@
       </c>
     </row>
     <row r="11" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>3</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="31" t="s">
         <v>776</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="42"/>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
-      <c r="N11" s="10">
-        <v>1</v>
-      </c>
-      <c r="O11" s="10"/>
+      <c r="N11" s="9">
+        <v>1</v>
+      </c>
+      <c r="O11" s="9"/>
       <c r="Q11" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -11635,21 +11854,21 @@
       </c>
     </row>
     <row r="12" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>4</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="32" t="s">
         <v>777</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="42"/>
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
       <c r="H12" s="42"/>
-      <c r="N12" s="10">
-        <v>1</v>
-      </c>
-      <c r="O12" s="10"/>
+      <c r="N12" s="9">
+        <v>1</v>
+      </c>
+      <c r="O12" s="9"/>
       <c r="Q12" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -11664,21 +11883,21 @@
       </c>
     </row>
     <row r="13" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <v>5</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="32" t="s">
         <v>778</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
       <c r="H13" s="42"/>
-      <c r="N13" s="10">
-        <v>1</v>
-      </c>
-      <c r="O13" s="10"/>
+      <c r="N13" s="9">
+        <v>1</v>
+      </c>
+      <c r="O13" s="9"/>
       <c r="Q13" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -11693,21 +11912,21 @@
       </c>
     </row>
     <row r="14" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="26">
+      <c r="B14" s="25">
         <v>6</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="33" t="s">
         <v>779</v>
       </c>
-      <c r="D14" s="23"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
       <c r="G14" s="42"/>
       <c r="H14" s="42"/>
-      <c r="N14" s="10">
-        <v>1</v>
-      </c>
-      <c r="O14" s="10"/>
+      <c r="N14" s="9">
+        <v>1</v>
+      </c>
+      <c r="O14" s="9"/>
       <c r="Q14" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -11716,27 +11935,27 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="S14" s="32" t="str">
+      <c r="S14" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="26">
+      <c r="B15" s="25">
         <v>7</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="33" t="s">
         <v>780</v>
       </c>
-      <c r="D15" s="23"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
       <c r="G15" s="42"/>
       <c r="H15" s="42"/>
-      <c r="N15" s="10">
-        <v>1</v>
-      </c>
-      <c r="O15" s="10"/>
+      <c r="N15" s="9">
+        <v>1</v>
+      </c>
+      <c r="O15" s="9"/>
       <c r="Q15" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -11751,21 +11970,21 @@
       </c>
     </row>
     <row r="16" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="26">
+      <c r="B16" s="25">
         <v>8</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="33" t="s">
         <v>781</v>
       </c>
-      <c r="D16" s="23"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="42"/>
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
       <c r="H16" s="42"/>
-      <c r="N16" s="10">
-        <v>1</v>
-      </c>
-      <c r="O16" s="10"/>
+      <c r="N16" s="9">
+        <v>1</v>
+      </c>
+      <c r="O16" s="9"/>
       <c r="Q16" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -11782,11 +12001,11 @@
     <row r="17" spans="14:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="14:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ls8kcXzEfysCyMwG/Bghjml6dzbC5GWQVS/WW91Hm6WtDb47JWG+IorZigD4lYZoEfew8+0T0aso39G/4tZL7g==" saltValue="9KuGCdv22rG66jzsI+vGMA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4jlbzBTBzfV/PGKd4+uDBhzxO8c304g31gGC+i3BAx42RaCkxLblIsQ5CIjYIQEbG7pnla43aANpvRhuFJFq5A==" saltValue="dYBEHRLVvM7kflNkXEfa8A==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="D19" name="Range1_1_1"/>
     <protectedRange sqref="D9:D11 D14" name="Range1_2"/>

</xml_diff>